<commit_message>
negative score adjustment added
</commit_message>
<xml_diff>
--- a/compile/data/weighted_adjustment.xlsx
+++ b/compile/data/weighted_adjustment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\group\compile\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC19CD1-1F3D-453C-99CA-6A30B12E0658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D90A481-392E-4945-A4BE-E633CA125A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8268" yWindow="1824" windowWidth="17280" windowHeight="8916" firstSheet="3" activeTab="5" xr2:uid="{FD519D9B-FD8C-4B05-8A2B-BFB2B0A3DB28}"/>
+    <workbookView xWindow="348" yWindow="1656" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="6" xr2:uid="{FD519D9B-FD8C-4B05-8A2B-BFB2B0A3DB28}"/>
   </bookViews>
   <sheets>
     <sheet name="industry" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="physical_channel" sheetId="4" r:id="rId4"/>
     <sheet name="lead_source" sheetId="5" r:id="rId5"/>
     <sheet name="designation" sheetId="6" r:id="rId6"/>
+    <sheet name="negative_score" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>weightage</t>
   </si>
@@ -313,6 +314,12 @@
   </si>
   <si>
     <t>Director</t>
+  </si>
+  <si>
+    <t>competitor</t>
+  </si>
+  <si>
+    <t>no competitor</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F4B3E4-2AA4-42DF-A18B-2369BF556360}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1137,4 +1144,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF780DE-784D-4A69-8B98-E103B0FEB401}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update weighted adjustment excel
</commit_message>
<xml_diff>
--- a/compile/data/weighted_adjustment.xlsx
+++ b/compile/data/weighted_adjustment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20ACC744-7FA0-4588-B0A9-F48B9F0CF726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4B1D5A-C060-4B1E-B404-382ACD9CD39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{FD519D9B-FD8C-4B05-8A2B-BFB2B0A3DB28}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <definedName name="solver_eng" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="8" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="8" hidden="1">'scoring adjustment'!$N$17</definedName>
+    <definedName name="solver_opt" localSheetId="8" hidden="1">'scoring adjustment'!$J$3</definedName>
     <definedName name="solver_typ" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="131">
   <si>
     <t>weightage</t>
   </si>
@@ -65,30 +65,18 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>Service logistics</t>
-  </si>
-  <si>
     <t>Manufacturing</t>
   </si>
   <si>
     <t>Chemical and Energy</t>
   </si>
   <si>
-    <t>Life Sciences and Healthcare</t>
-  </si>
-  <si>
     <t>Automotive</t>
   </si>
   <si>
-    <t>Engineering</t>
-  </si>
-  <si>
     <t>Distributor</t>
   </si>
   <si>
-    <t xml:space="preserve">Service  </t>
-  </si>
-  <si>
     <t>&gt; 6 months</t>
   </si>
   <si>
@@ -137,18 +125,12 @@
     <t>Secretary</t>
   </si>
   <si>
-    <t>Cleaner</t>
-  </si>
-  <si>
     <t>Director</t>
   </si>
   <si>
     <t>Industry</t>
   </si>
   <si>
-    <t>Weightage</t>
-  </si>
-  <si>
     <t>Positive score</t>
   </si>
   <si>
@@ -167,27 +149,9 @@
     <t>Employee Count</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt; 100 </t>
-  </si>
-  <si>
-    <t>50 - 100</t>
-  </si>
-  <si>
-    <t>1 till 50</t>
-  </si>
-  <si>
     <t>Total Potential Revenue/Month</t>
   </si>
   <si>
-    <t>&gt; 1000</t>
-  </si>
-  <si>
-    <t>500 - 1000</t>
-  </si>
-  <si>
-    <t>100 - 500</t>
-  </si>
-  <si>
     <t>&lt; 100</t>
   </si>
   <si>
@@ -281,27 +245,15 @@
     <t>Insurance</t>
   </si>
   <si>
-    <t>Signup Pages</t>
-  </si>
-  <si>
     <t>Facebook</t>
   </si>
   <si>
     <t>Ex Database</t>
   </si>
   <si>
-    <t>Content Blogs</t>
-  </si>
-  <si>
-    <t>Procured from Market</t>
-  </si>
-  <si>
     <t>Exhibition</t>
   </si>
   <si>
-    <t>Weightage 8</t>
-  </si>
-  <si>
     <t>Pos Laju</t>
   </si>
   <si>
@@ -399,6 +351,102 @@
   </si>
   <si>
     <t>0xxxxxxx9</t>
+  </si>
+  <si>
+    <t>+60132889261</t>
+  </si>
+  <si>
+    <t>013465r566</t>
+  </si>
+  <si>
+    <t>&lt;10</t>
+  </si>
+  <si>
+    <t>10 - 49</t>
+  </si>
+  <si>
+    <t>50 - 249</t>
+  </si>
+  <si>
+    <t>&gt; 249</t>
+  </si>
+  <si>
+    <t>100 - 999</t>
+  </si>
+  <si>
+    <t>1000 - 9999</t>
+  </si>
+  <si>
+    <t>10000 - 99999</t>
+  </si>
+  <si>
+    <t>&gt; 100000</t>
+  </si>
+  <si>
+    <t>Subscription based</t>
+  </si>
+  <si>
+    <t>On demand</t>
+  </si>
+  <si>
+    <t>E-Commerce</t>
+  </si>
+  <si>
+    <t>Logistic Services</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Pharmaceutical</t>
+  </si>
+  <si>
+    <t>Printing</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Signup Page</t>
+  </si>
+  <si>
+    <t>Landing page</t>
+  </si>
+  <si>
+    <t>Referrals</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>Market Data</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>Personal Assistant</t>
   </si>
 </sst>
 </file>
@@ -434,7 +482,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,8 +507,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -468,11 +522,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -482,10 +551,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A76A01-22F1-482E-9E77-71DAC060A196}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B3" sqref="B3:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,10 +888,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -825,7 +900,7 @@
       </c>
       <c r="B2">
         <f>'scoring adjustment'!C3</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -851,37 +926,37 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>'scoring adjustment'!A6</f>
-        <v>Technology</v>
+        <v>E-Commerce</v>
       </c>
       <c r="B5">
         <f>'scoring adjustment'!C6</f>
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>'scoring adjustment'!A7</f>
-        <v>Service logistics</v>
+        <v>Distributor</v>
       </c>
       <c r="B6">
         <f>'scoring adjustment'!C7</f>
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>'scoring adjustment'!A8</f>
-        <v>Manufacturing</v>
+        <v>Logistic Services</v>
       </c>
       <c r="B7">
         <f>'scoring adjustment'!C8</f>
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>'scoring adjustment'!A9</f>
-        <v>Chemical and Energy</v>
+        <v>Healthcare</v>
       </c>
       <c r="B8">
         <f>'scoring adjustment'!C9</f>
@@ -891,7 +966,7 @@
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>'scoring adjustment'!A10</f>
-        <v>Distributor</v>
+        <v>Pharmaceutical</v>
       </c>
       <c r="B9">
         <f>'scoring adjustment'!C10</f>
@@ -901,59 +976,121 @@
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>'scoring adjustment'!A11</f>
-        <v>Life Sciences and Healthcare</v>
+        <v>Printing</v>
       </c>
       <c r="B10">
         <f>'scoring adjustment'!C11</f>
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>'scoring adjustment'!A12</f>
-        <v>Automotive</v>
+        <v>Technology</v>
       </c>
       <c r="B11">
         <f>'scoring adjustment'!C12</f>
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>'scoring adjustment'!A13</f>
-        <v>Engineering</v>
+        <v>Manufacturing</v>
       </c>
       <c r="B12">
         <f>'scoring adjustment'!C13</f>
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>'scoring adjustment'!A14</f>
-        <v xml:space="preserve">Service  </v>
+        <v>Automotive</v>
       </c>
       <c r="B13">
         <f>'scoring adjustment'!C14</f>
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>'scoring adjustment'!A15</f>
-        <v>Others</v>
+        <v>Food</v>
       </c>
       <c r="B14">
         <f>'scoring adjustment'!C15</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="str">
+        <f>'scoring adjustment'!A16</f>
+        <v>Law</v>
+      </c>
+      <c r="B15">
+        <f>'scoring adjustment'!C16</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="str">
+        <f>'scoring adjustment'!A17</f>
+        <v>Agriculture</v>
+      </c>
+      <c r="B16">
+        <f>'scoring adjustment'!C17</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="str">
+        <f>'scoring adjustment'!A18</f>
+        <v>Chemical and Energy</v>
+      </c>
+      <c r="B17">
+        <f>'scoring adjustment'!C18</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="str">
+        <f>'scoring adjustment'!A19</f>
+        <v>Banking</v>
+      </c>
+      <c r="B18">
+        <f>'scoring adjustment'!C19</f>
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15">
-        <v>-100</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="str">
+        <f>'scoring adjustment'!A20</f>
+        <v>Construction</v>
+      </c>
+      <c r="B19">
+        <f>'scoring adjustment'!C20</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="str">
+        <f>'scoring adjustment'!A21</f>
+        <v>Insurance</v>
+      </c>
+      <c r="B20">
+        <f>'scoring adjustment'!C21</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="str">
+        <f>'scoring adjustment'!A22</f>
+        <v>Others</v>
+      </c>
+      <c r="B21">
+        <f>'scoring adjustment'!C22</f>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -981,7 +1118,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>-50</v>
@@ -989,7 +1126,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>-100</v>
@@ -997,7 +1134,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -1005,7 +1142,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -1045,20 +1182,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB39EB3-5C8D-47CC-9F86-693F4D81C503}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1066,13 +1203,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>'scoring adjustment'!C17</f>
+        <f>'scoring adjustment'!C25</f>
         <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>'scoring adjustment'!A18</f>
+        <f>'scoring adjustment'!A26</f>
         <v>B2B</v>
       </c>
       <c r="B3">
@@ -1081,32 +1218,52 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>'scoring adjustment'!A19</f>
+        <f>'scoring adjustment'!A27</f>
         <v>B2C</v>
       </c>
       <c r="B4">
-        <f>'scoring adjustment'!C19</f>
+        <f>'scoring adjustment'!C27</f>
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>'scoring adjustment'!A20</f>
-        <v>Non-profit</v>
+        <f>'scoring adjustment'!A28</f>
+        <v>Subscription based</v>
       </c>
       <c r="B5">
-        <f>'scoring adjustment'!C20</f>
-        <v>-50</v>
+        <f>'scoring adjustment'!C28</f>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>'scoring adjustment'!A21</f>
+        <f>'scoring adjustment'!A29</f>
+        <v>On demand</v>
+      </c>
+      <c r="B6">
+        <f>'scoring adjustment'!C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>'scoring adjustment'!A30</f>
+        <v>Non-profit</v>
+      </c>
+      <c r="B7">
+        <f>'scoring adjustment'!C30</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>'scoring adjustment'!A31</f>
         <v>Others</v>
       </c>
-      <c r="B6">
-        <f>'scoring adjustment'!C21</f>
-        <v>-50</v>
+      <c r="B8">
+        <f>'scoring adjustment'!C31</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1116,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0957A0A-2F34-4B4E-B07C-7D49062D6D9E}">
-  <dimension ref="C1:D10"/>
+  <dimension ref="C1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C14" sqref="C14:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1129,10 +1286,10 @@
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.3">
@@ -1140,87 +1297,117 @@
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <f>'scoring adjustment'!G17</f>
+        <f>'scoring adjustment'!O3</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C3" t="str">
-        <f>'scoring adjustment'!E18</f>
-        <v>Signup Pages</v>
+        <f>'scoring adjustment'!M4</f>
+        <v>Signup Page</v>
       </c>
       <c r="D3" s="3">
-        <f>'scoring adjustment'!G18</f>
+        <f>'scoring adjustment'!O4</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4" t="str">
-        <f>'scoring adjustment'!E19</f>
-        <v>Exhibition</v>
+        <f>'scoring adjustment'!M5</f>
+        <v>Landing page</v>
       </c>
       <c r="D4" s="3">
-        <f>'scoring adjustment'!G19</f>
+        <f>'scoring adjustment'!O5</f>
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" t="str">
-        <f>'scoring adjustment'!E20</f>
-        <v>Facebook</v>
+        <f>'scoring adjustment'!M6</f>
+        <v>Exhibition</v>
       </c>
       <c r="D5" s="3">
-        <f>'scoring adjustment'!G20</f>
-        <v>70</v>
+        <f>'scoring adjustment'!O6</f>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="str">
-        <f>'scoring adjustment'!E21</f>
-        <v>Twitter</v>
+        <f>'scoring adjustment'!M7</f>
+        <v>Referrals</v>
       </c>
       <c r="D6" s="3">
-        <f>'scoring adjustment'!G21</f>
-        <v>70</v>
+        <f>'scoring adjustment'!O7</f>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" t="str">
-        <f>'scoring adjustment'!E22</f>
-        <v>Ex Database</v>
+        <f>'scoring adjustment'!M8</f>
+        <v>LinkedIn</v>
       </c>
       <c r="D7" s="3">
-        <f>'scoring adjustment'!G22</f>
-        <v>50</v>
+        <f>'scoring adjustment'!O8</f>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" t="str">
-        <f>'scoring adjustment'!E23</f>
-        <v>Content Blogs</v>
+        <f>'scoring adjustment'!M9</f>
+        <v>Facebook</v>
       </c>
       <c r="D8" s="3">
-        <f>'scoring adjustment'!G23</f>
-        <v>50</v>
+        <f>'scoring adjustment'!O9</f>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9" t="str">
-        <f>'scoring adjustment'!E24</f>
-        <v>Procured from Market</v>
+        <f>'scoring adjustment'!M10</f>
+        <v>Twitter</v>
       </c>
       <c r="D9" s="3">
-        <f>'scoring adjustment'!G24</f>
-        <v>-10</v>
+        <f>'scoring adjustment'!O10</f>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" t="str">
-        <f>'scoring adjustment'!E25</f>
+        <f>'scoring adjustment'!M11</f>
+        <v>Blog</v>
+      </c>
+      <c r="D10" s="3">
+        <f>'scoring adjustment'!O11</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C11" t="str">
+        <f>'scoring adjustment'!M12</f>
+        <v>Ex Database</v>
+      </c>
+      <c r="D11" s="3">
+        <f>'scoring adjustment'!O12</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="str">
+        <f>'scoring adjustment'!M13</f>
+        <v>Market Data</v>
+      </c>
+      <c r="D12" s="3">
+        <f>'scoring adjustment'!O13</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="str">
+        <f>'scoring adjustment'!M14</f>
         <v>Others</v>
       </c>
-      <c r="D10" s="3">
-        <f>'scoring adjustment'!G25</f>
+      <c r="D13" s="3">
+        <f>'scoring adjustment'!O14</f>
         <v>-10</v>
       </c>
     </row>
@@ -1231,20 +1418,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F4B3E4-2AA4-42DF-A18B-2369BF556360}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1252,97 +1439,127 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <f>'scoring adjustment'!K17</f>
+        <f>'scoring adjustment'!G3</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>'scoring adjustment'!I18</f>
+        <f>'scoring adjustment'!E4</f>
         <v>CEO</v>
       </c>
       <c r="B3" s="3">
-        <f>'scoring adjustment'!K18</f>
+        <f>'scoring adjustment'!G4</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>'scoring adjustment'!I19</f>
+        <f>'scoring adjustment'!E5</f>
         <v>Sales</v>
       </c>
       <c r="B4" s="3">
-        <f>'scoring adjustment'!K19</f>
+        <f>'scoring adjustment'!G5</f>
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>'scoring adjustment'!I20</f>
+        <f>'scoring adjustment'!E6</f>
         <v>Logistics</v>
       </c>
       <c r="B5" s="3">
-        <f>'scoring adjustment'!K20</f>
+        <f>'scoring adjustment'!G6</f>
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>'scoring adjustment'!I21</f>
+        <f>'scoring adjustment'!E7</f>
         <v>Director</v>
       </c>
       <c r="B6" s="3">
-        <f>'scoring adjustment'!K21</f>
+        <f>'scoring adjustment'!G7</f>
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f>'scoring adjustment'!I22</f>
-        <v>Executive</v>
+        <f>'scoring adjustment'!E8</f>
+        <v>Manager</v>
       </c>
       <c r="B7" s="3">
-        <f>'scoring adjustment'!K22</f>
+        <f>'scoring adjustment'!G8</f>
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>'scoring adjustment'!I23</f>
-        <v>Secretary</v>
+        <f>'scoring adjustment'!E9</f>
+        <v>Accountant</v>
       </c>
       <c r="B8" s="3">
-        <f>'scoring adjustment'!K23</f>
+        <f>'scoring adjustment'!G9</f>
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>'scoring adjustment'!I24</f>
-        <v>Technician</v>
+        <f>'scoring adjustment'!E10</f>
+        <v>Business Analyst</v>
       </c>
       <c r="B9" s="3">
-        <f>'scoring adjustment'!K24</f>
-        <v>50</v>
+        <f>'scoring adjustment'!G10</f>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>'scoring adjustment'!I25</f>
-        <v>Cleaner</v>
+        <f>'scoring adjustment'!E11</f>
+        <v>Executive</v>
       </c>
       <c r="B10" s="3">
-        <f>'scoring adjustment'!K25</f>
-        <v>0</v>
+        <f>'scoring adjustment'!G11</f>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f>'scoring adjustment'!I26</f>
+        <f>'scoring adjustment'!E12</f>
+        <v>Secretary</v>
+      </c>
+      <c r="B11" s="3">
+        <f>'scoring adjustment'!G12</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>'scoring adjustment'!E13</f>
+        <v>Personal Assistant</v>
+      </c>
+      <c r="B12" s="3">
+        <f>'scoring adjustment'!G13</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>'scoring adjustment'!E14</f>
+        <v>Technician</v>
+      </c>
+      <c r="B13" s="3">
+        <f>'scoring adjustment'!G14</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>'scoring adjustment'!E15</f>
         <v>Others</v>
       </c>
-      <c r="B11" s="3">
-        <f>'scoring adjustment'!K26</f>
+      <c r="B14" s="3">
+        <f>'scoring adjustment'!G15</f>
         <v>0</v>
       </c>
     </row>
@@ -1363,10 +1580,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1374,107 +1591,107 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>'scoring adjustment'!O17</f>
+        <f>'scoring adjustment'!K3</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>'scoring adjustment'!M18</f>
+        <f>'scoring adjustment'!I4</f>
         <v>Pos Laju</v>
       </c>
       <c r="B3">
-        <f>'scoring adjustment'!O18</f>
+        <f>'scoring adjustment'!K4</f>
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>'scoring adjustment'!M19</f>
+        <f>'scoring adjustment'!I5</f>
         <v>Gdex</v>
       </c>
       <c r="B4">
-        <f>'scoring adjustment'!O19</f>
+        <f>'scoring adjustment'!K5</f>
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>'scoring adjustment'!M20</f>
+        <f>'scoring adjustment'!I6</f>
         <v>Fedex</v>
       </c>
       <c r="B5">
-        <f>'scoring adjustment'!O20</f>
+        <f>'scoring adjustment'!K6</f>
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>'scoring adjustment'!M21</f>
+        <f>'scoring adjustment'!I7</f>
         <v>J&amp;T</v>
       </c>
       <c r="B6">
-        <f>'scoring adjustment'!O21</f>
+        <f>'scoring adjustment'!K7</f>
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
-        <f>'scoring adjustment'!M22</f>
+        <f>'scoring adjustment'!I8</f>
         <v>Citylink</v>
       </c>
       <c r="B7">
-        <f>'scoring adjustment'!O22</f>
+        <f>'scoring adjustment'!K8</f>
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>'scoring adjustment'!M23</f>
+        <f>'scoring adjustment'!I9</f>
         <v>Easyparcel</v>
       </c>
       <c r="B8">
-        <f>'scoring adjustment'!O23</f>
+        <f>'scoring adjustment'!K9</f>
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>'scoring adjustment'!M24</f>
+        <f>'scoring adjustment'!I10</f>
         <v>Pgeon</v>
       </c>
       <c r="B9">
-        <f>'scoring adjustment'!O24</f>
+        <f>'scoring adjustment'!K10</f>
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>'scoring adjustment'!M25</f>
+        <f>'scoring adjustment'!I11</f>
         <v>Ninjavan</v>
       </c>
       <c r="B10">
-        <f>'scoring adjustment'!O25</f>
+        <f>'scoring adjustment'!K11</f>
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f>'scoring adjustment'!M26</f>
+        <f>'scoring adjustment'!I12</f>
         <v>Lalamove</v>
       </c>
       <c r="B11">
-        <f>'scoring adjustment'!O26</f>
+        <f>'scoring adjustment'!K12</f>
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f>'scoring adjustment'!M27</f>
+        <f>'scoring adjustment'!I13</f>
         <v>Others</v>
       </c>
       <c r="B12">
-        <f>'scoring adjustment'!O27</f>
+        <f>'scoring adjustment'!K13</f>
         <v>100</v>
       </c>
     </row>
@@ -1488,7 +1705,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1498,10 +1715,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1509,47 +1726,47 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>'scoring adjustment'!C31</f>
+        <f>'scoring adjustment'!C39</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
-        <f>'scoring adjustment'!A32</f>
+        <f>'scoring adjustment'!A40</f>
         <v>All Null</v>
       </c>
       <c r="B3">
-        <f>'scoring adjustment'!C32</f>
+        <f>'scoring adjustment'!C40</f>
         <v>-100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
-        <f>'scoring adjustment'!A33</f>
+        <f>'scoring adjustment'!A41</f>
         <v>Null email</v>
       </c>
       <c r="B4">
-        <f>'scoring adjustment'!C33</f>
+        <f>'scoring adjustment'!C41</f>
         <v>-5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
-        <f>'scoring adjustment'!A34</f>
+        <f>'scoring adjustment'!A42</f>
         <v>Null phone no.</v>
       </c>
       <c r="B5">
-        <f>'scoring adjustment'!C34</f>
-        <v>-50</v>
+        <f>'scoring adjustment'!C42</f>
+        <v>-20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
-        <f>'scoring adjustment'!A35</f>
+        <f>'scoring adjustment'!A43</f>
         <v>Have both</v>
       </c>
       <c r="B6">
-        <f>'scoring adjustment'!C35</f>
+        <f>'scoring adjustment'!C43</f>
         <v>0</v>
       </c>
     </row>
@@ -1560,16 +1777,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7D6719-ECED-4193-8F1E-6CF4287CC736}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.109375" customWidth="1"/>
     <col min="6" max="6" width="11.21875" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
@@ -1579,71 +1797,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="8">
+      <c r="J3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="12">
         <v>0.2</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0.05</v>
-      </c>
       <c r="M3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="4">
+        <v>37</v>
+      </c>
+      <c r="O3" s="12">
         <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="7">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="8">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4">
+        <v>66</v>
+      </c>
+      <c r="K4" s="7">
         <v>100</v>
       </c>
       <c r="M4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4">
+        <v>121</v>
+      </c>
+      <c r="O4" s="7">
         <v>100</v>
       </c>
     </row>
@@ -1651,667 +1870,793 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="G5" s="7">
+        <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5">
-        <v>50</v>
+        <v>67</v>
+      </c>
+      <c r="K5" s="7">
+        <v>100</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5">
-        <v>80</v>
+        <v>122</v>
+      </c>
+      <c r="O5" s="7">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8">
-        <v>80</v>
+        <v>111</v>
+      </c>
+      <c r="C6" s="7">
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6">
-        <v>-50</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K6">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G6" s="7">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="7">
+        <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="O6" s="14">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="8">
-        <v>80</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7">
-        <v>-100</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>-10</v>
+        <v>23</v>
+      </c>
+      <c r="G7" s="7">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="7">
+        <v>80</v>
       </c>
       <c r="M7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O7">
-        <v>20</v>
+        <v>123</v>
+      </c>
+      <c r="O7" s="7">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="8">
+        <v>112</v>
+      </c>
+      <c r="C8" s="7">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="7">
+        <v>80</v>
+      </c>
+      <c r="I8" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="7">
+        <v>80</v>
+      </c>
+      <c r="M8" t="s">
+        <v>124</v>
+      </c>
+      <c r="O8" s="7">
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="8">
-        <v>80</v>
+        <v>113</v>
+      </c>
+      <c r="C9" s="7">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="7">
+        <v>80</v>
+      </c>
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="7">
+        <v>80</v>
+      </c>
+      <c r="M9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9" s="7">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8">
-        <v>80</v>
+        <v>114</v>
+      </c>
+      <c r="C10" s="7">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" s="7">
+        <v>80</v>
+      </c>
+      <c r="I10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="7">
+        <v>80</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="7">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="8">
+        <v>115</v>
+      </c>
+      <c r="C11" s="7">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="7">
+        <v>70</v>
+      </c>
+      <c r="I11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" s="7">
+        <v>80</v>
+      </c>
+      <c r="M11" t="s">
+        <v>125</v>
+      </c>
+      <c r="O11" s="7">
         <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="7">
+        <v>80</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="7">
         <v>60</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" s="7">
+        <v>80</v>
+      </c>
+      <c r="M12" t="s">
+        <v>64</v>
+      </c>
+      <c r="O12" s="7">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="8">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G13" s="7">
         <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+      <c r="K13" s="7">
+        <v>100</v>
+      </c>
+      <c r="M13" t="s">
+        <v>126</v>
+      </c>
+      <c r="O13" s="7">
+        <v>-10</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="8">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="C14" s="7">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="7">
+        <v>50</v>
+      </c>
+      <c r="M14" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" s="7">
+        <v>-10</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="8">
+        <v>116</v>
+      </c>
+      <c r="C15" s="7">
+        <v>80</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7">
+        <v>100</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="I26" t="s">
+        <v>108</v>
+      </c>
+      <c r="K26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="7">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27">
         <v>50</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="I27" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="K27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="7">
+        <v>10</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="K28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="7">
+        <v>-50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="10">
+        <f>C3+G25+K25+C25+O3+G3+K3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I39" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="J39" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="7">
+        <v>-100</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
         <v>53</v>
       </c>
-      <c r="G17" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="I17" s="4" t="s">
+      <c r="J40" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="4" t="s">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="9">
+        <v>-5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41">
+        <v>-20</v>
+      </c>
+      <c r="I41" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="M17" s="4" t="s">
+      <c r="J41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="7">
+        <v>-20</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42">
+        <v>-50</v>
+      </c>
+      <c r="I42" t="s">
         <v>57</v>
       </c>
-      <c r="N17" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="O17" s="8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="8">
-        <v>100</v>
-      </c>
-      <c r="E18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="8">
-        <v>100</v>
-      </c>
-      <c r="I18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="8">
-        <v>100</v>
-      </c>
-      <c r="M18" t="s">
-        <v>82</v>
-      </c>
-      <c r="O18" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="8">
-        <v>80</v>
-      </c>
-      <c r="E19" t="s">
-        <v>80</v>
-      </c>
-      <c r="G19" s="8">
-        <v>100</v>
-      </c>
-      <c r="I19" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="8">
-        <v>100</v>
-      </c>
-      <c r="M19" t="s">
-        <v>83</v>
-      </c>
-      <c r="O19" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="8">
-        <v>-50</v>
-      </c>
-      <c r="E20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="8">
-        <v>70</v>
-      </c>
-      <c r="I20" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="8">
-        <v>100</v>
-      </c>
-      <c r="M20" t="s">
-        <v>85</v>
-      </c>
-      <c r="O20" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="8">
-        <v>-50</v>
-      </c>
-      <c r="E21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="8">
-        <v>70</v>
-      </c>
-      <c r="I21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="8">
-        <v>100</v>
-      </c>
-      <c r="M21" t="s">
-        <v>84</v>
-      </c>
-      <c r="O21" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E22" t="s">
+      <c r="J42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="7">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43">
+        <v>-100</v>
+      </c>
+      <c r="I43" t="s">
+        <v>59</v>
+      </c>
+      <c r="J43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="7">
+        <f t="shared" ref="B45:B54" si="0">LEN(A45)</f>
+        <v>17</v>
+      </c>
+      <c r="D45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>77</v>
       </c>
-      <c r="G22" s="8">
-        <v>50</v>
-      </c>
-      <c r="I22" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="8">
-        <v>80</v>
-      </c>
-      <c r="M22" t="s">
-        <v>86</v>
-      </c>
-      <c r="O22" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
-        <v>78</v>
-      </c>
-      <c r="G23" s="8">
-        <v>50</v>
-      </c>
-      <c r="I23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="8">
-        <v>80</v>
-      </c>
-      <c r="M23" t="s">
-        <v>87</v>
-      </c>
-      <c r="O23" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="8">
-        <v>-10</v>
-      </c>
-      <c r="I24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="8">
-        <v>50</v>
-      </c>
-      <c r="M24" t="s">
-        <v>88</v>
-      </c>
-      <c r="O24" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
-        <v>91</v>
-      </c>
-      <c r="G25" s="8">
-        <v>-10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K25" s="8">
-        <v>0</v>
-      </c>
-      <c r="M25" t="s">
-        <v>89</v>
-      </c>
-      <c r="O25" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I26" t="s">
-        <v>91</v>
-      </c>
-      <c r="K26" s="8">
-        <v>0</v>
-      </c>
-      <c r="M26" t="s">
-        <v>90</v>
-      </c>
-      <c r="O26" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27">
-        <f>C3+G3+K3+O3+C17+G17+K17+O17</f>
-        <v>1</v>
-      </c>
-      <c r="M27" t="s">
-        <v>91</v>
-      </c>
-      <c r="O27" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="8">
-        <v>1</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="8">
-        <v>-100</v>
-      </c>
-      <c r="E32" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="8">
-        <v>-5</v>
-      </c>
-      <c r="E33" t="s">
-        <v>67</v>
-      </c>
-      <c r="F33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="8">
-        <v>-50</v>
-      </c>
-      <c r="E34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="8">
-        <v>0</v>
-      </c>
-      <c r="E35" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="8">
-        <f t="shared" ref="B37:B46" si="0">LEN(A37)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38">
+      <c r="B46">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39">
+      <c r="D46" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>95</v>
-      </c>
-      <c r="B40">
+      <c r="D47" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47">
+        <f>LEN(D47)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41">
+      <c r="D48" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48">
+        <f>LEN(D48)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" s="8">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>100</v>
-      </c>
-      <c r="B45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>101</v>
-      </c>
-      <c r="B46">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>102</v>
-      </c>
-      <c r="B47">
-        <f>LEN(A47)</f>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55">
+        <f>LEN(A55)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" s="8">
-        <f t="shared" ref="B48:B58" si="1">LEN(A48)</f>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" s="7">
+        <f t="shared" ref="B56:B66" si="1">LEN(A56)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>105</v>
-      </c>
-      <c r="B49">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>107</v>
-      </c>
-      <c r="B51">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>108</v>
-      </c>
-      <c r="B52">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" s="8">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" s="7">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>114</v>
-      </c>
-      <c r="B57">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" s="8">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="7">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Added scoring adjustment for last_created
</commit_message>
<xml_diff>
--- a/compile/data/weighted_adjustment.xlsx
+++ b/compile/data/weighted_adjustment.xlsx
@@ -8,30 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4B1D5A-C060-4B1E-B404-382ACD9CD39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34B439B-5DBA-4C83-AAAB-D99D6376E6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="8" xr2:uid="{FD519D9B-FD8C-4B05-8A2B-BFB2B0A3DB28}"/>
   </bookViews>
   <sheets>
     <sheet name="industry" sheetId="1" r:id="rId1"/>
     <sheet name="creation_date" sheetId="2" r:id="rId2"/>
-    <sheet name="employee_count" sheetId="3" r:id="rId3"/>
-    <sheet name="physical_channel" sheetId="4" r:id="rId4"/>
-    <sheet name="lead_source" sheetId="5" r:id="rId5"/>
-    <sheet name="designation" sheetId="6" r:id="rId6"/>
-    <sheet name="competitor" sheetId="9" r:id="rId7"/>
-    <sheet name="negative_score" sheetId="7" r:id="rId8"/>
-    <sheet name="scoring adjustment" sheetId="8" r:id="rId9"/>
+    <sheet name="scoring adjustment" sheetId="8" r:id="rId3"/>
+    <sheet name="employee_count" sheetId="3" r:id="rId4"/>
+    <sheet name="physical_channel" sheetId="4" r:id="rId5"/>
+    <sheet name="lead_source" sheetId="5" r:id="rId6"/>
+    <sheet name="designation" sheetId="6" r:id="rId7"/>
+    <sheet name="competitor" sheetId="9" r:id="rId8"/>
+    <sheet name="contact_score" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="8" hidden="1">'scoring adjustment'!$C$3</definedName>
-    <definedName name="solver_eng" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="8" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="8" hidden="1">'scoring adjustment'!$J$3</definedName>
-    <definedName name="solver_typ" localSheetId="8" hidden="1">3</definedName>
-    <definedName name="solver_val" localSheetId="8" hidden="1">1</definedName>
-    <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'scoring adjustment'!$C$3</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'scoring adjustment'!$J$3</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="127">
   <si>
     <t>weightage</t>
   </si>
@@ -75,18 +75,6 @@
   </si>
   <si>
     <t>Distributor</t>
-  </si>
-  <si>
-    <t>&gt; 6 months</t>
-  </si>
-  <si>
-    <t>&gt; 12 months</t>
-  </si>
-  <si>
-    <t>3-6 months</t>
-  </si>
-  <si>
-    <t>&lt; 3 months</t>
   </si>
   <si>
     <t>numeric</t>
@@ -453,7 +441,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +465,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -541,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -561,6 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,10 +884,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -955,81 +951,81 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
-        <f>'scoring adjustment'!A9</f>
+        <f>'scoring adjustment'!A10</f>
         <v>Healthcare</v>
       </c>
       <c r="B8">
-        <f>'scoring adjustment'!C9</f>
+        <f>'scoring adjustment'!C10</f>
         <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
-        <f>'scoring adjustment'!A10</f>
+        <f>'scoring adjustment'!A11</f>
         <v>Pharmaceutical</v>
       </c>
       <c r="B9">
-        <f>'scoring adjustment'!C10</f>
+        <f>'scoring adjustment'!C11</f>
         <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
-        <f>'scoring adjustment'!A11</f>
+        <f>'scoring adjustment'!A12</f>
         <v>Printing</v>
       </c>
       <c r="B10">
-        <f>'scoring adjustment'!C11</f>
+        <f>'scoring adjustment'!C12</f>
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f>'scoring adjustment'!A12</f>
+        <f>'scoring adjustment'!A13</f>
         <v>Technology</v>
       </c>
       <c r="B11">
-        <f>'scoring adjustment'!C12</f>
+        <f>'scoring adjustment'!C13</f>
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f>'scoring adjustment'!A13</f>
+        <f>'scoring adjustment'!A14</f>
         <v>Manufacturing</v>
       </c>
       <c r="B12">
-        <f>'scoring adjustment'!C13</f>
+        <f>'scoring adjustment'!C14</f>
         <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
-        <f>'scoring adjustment'!A14</f>
+        <f>'scoring adjustment'!A15</f>
         <v>Automotive</v>
       </c>
       <c r="B13">
-        <f>'scoring adjustment'!C14</f>
+        <f>'scoring adjustment'!C15</f>
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
-        <f>'scoring adjustment'!A15</f>
+        <f>'scoring adjustment'!A16</f>
         <v>Food</v>
       </c>
       <c r="B14">
-        <f>'scoring adjustment'!C15</f>
+        <f>'scoring adjustment'!C16</f>
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
-        <f>'scoring adjustment'!A16</f>
+        <f>'scoring adjustment'!A9</f>
         <v>Law</v>
       </c>
       <c r="B15">
-        <f>'scoring adjustment'!C16</f>
+        <f>'scoring adjustment'!C9</f>
         <v>80</v>
       </c>
     </row>
@@ -1080,7 +1076,7 @@
       </c>
       <c r="B20">
         <f>'scoring adjustment'!C21</f>
-        <v>100</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1103,49 +1099,62 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>0.15</v>
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2">
+        <f>'scoring adjustment'!G39</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f>'scoring adjustment'!G40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <f>'scoring adjustment'!G41</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>90</v>
+      </c>
+      <c r="B5">
+        <f>'scoring adjustment'!G42</f>
         <v>-50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>89</v>
+      </c>
+      <c r="B6">
+        <f>'scoring adjustment'!G43</f>
         <v>-100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1169,618 +1178,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C4B6C5-2FF9-429D-B1B8-6831F1847B16}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB39EB3-5C8D-47CC-9F86-693F4D81C503}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>'scoring adjustment'!C25</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>'scoring adjustment'!A26</f>
-        <v>B2B</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>'scoring adjustment'!A27</f>
-        <v>B2C</v>
-      </c>
-      <c r="B4">
-        <f>'scoring adjustment'!C27</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>'scoring adjustment'!A28</f>
-        <v>Subscription based</v>
-      </c>
-      <c r="B5">
-        <f>'scoring adjustment'!C28</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>'scoring adjustment'!A29</f>
-        <v>On demand</v>
-      </c>
-      <c r="B6">
-        <f>'scoring adjustment'!C29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>'scoring adjustment'!A30</f>
-        <v>Non-profit</v>
-      </c>
-      <c r="B7">
-        <f>'scoring adjustment'!C30</f>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f>'scoring adjustment'!A31</f>
-        <v>Others</v>
-      </c>
-      <c r="B8">
-        <f>'scoring adjustment'!C31</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0957A0A-2F34-4B4E-B07C-7D49062D6D9E}">
-  <dimension ref="C1:D13"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="19.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <f>'scoring adjustment'!O3</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C3" t="str">
-        <f>'scoring adjustment'!M4</f>
-        <v>Signup Page</v>
-      </c>
-      <c r="D3" s="3">
-        <f>'scoring adjustment'!O4</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C4" t="str">
-        <f>'scoring adjustment'!M5</f>
-        <v>Landing page</v>
-      </c>
-      <c r="D4" s="3">
-        <f>'scoring adjustment'!O5</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C5" t="str">
-        <f>'scoring adjustment'!M6</f>
-        <v>Exhibition</v>
-      </c>
-      <c r="D5" s="3">
-        <f>'scoring adjustment'!O6</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C6" t="str">
-        <f>'scoring adjustment'!M7</f>
-        <v>Referrals</v>
-      </c>
-      <c r="D6" s="3">
-        <f>'scoring adjustment'!O7</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C7" t="str">
-        <f>'scoring adjustment'!M8</f>
-        <v>LinkedIn</v>
-      </c>
-      <c r="D7" s="3">
-        <f>'scoring adjustment'!O8</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C8" t="str">
-        <f>'scoring adjustment'!M9</f>
-        <v>Facebook</v>
-      </c>
-      <c r="D8" s="3">
-        <f>'scoring adjustment'!O9</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C9" t="str">
-        <f>'scoring adjustment'!M10</f>
-        <v>Twitter</v>
-      </c>
-      <c r="D9" s="3">
-        <f>'scoring adjustment'!O10</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C10" t="str">
-        <f>'scoring adjustment'!M11</f>
-        <v>Blog</v>
-      </c>
-      <c r="D10" s="3">
-        <f>'scoring adjustment'!O11</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C11" t="str">
-        <f>'scoring adjustment'!M12</f>
-        <v>Ex Database</v>
-      </c>
-      <c r="D11" s="3">
-        <f>'scoring adjustment'!O12</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C12" t="str">
-        <f>'scoring adjustment'!M13</f>
-        <v>Market Data</v>
-      </c>
-      <c r="D12" s="3">
-        <f>'scoring adjustment'!O13</f>
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="str">
-        <f>'scoring adjustment'!M14</f>
-        <v>Others</v>
-      </c>
-      <c r="D13" s="3">
-        <f>'scoring adjustment'!O14</f>
-        <v>-10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F4B3E4-2AA4-42DF-A18B-2369BF556360}">
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <f>'scoring adjustment'!G3</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>'scoring adjustment'!E4</f>
-        <v>CEO</v>
-      </c>
-      <c r="B3" s="3">
-        <f>'scoring adjustment'!G4</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>'scoring adjustment'!E5</f>
-        <v>Sales</v>
-      </c>
-      <c r="B4" s="3">
-        <f>'scoring adjustment'!G5</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>'scoring adjustment'!E6</f>
-        <v>Logistics</v>
-      </c>
-      <c r="B5" s="3">
-        <f>'scoring adjustment'!G6</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>'scoring adjustment'!E7</f>
-        <v>Director</v>
-      </c>
-      <c r="B6" s="3">
-        <f>'scoring adjustment'!G7</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>'scoring adjustment'!E8</f>
-        <v>Manager</v>
-      </c>
-      <c r="B7" s="3">
-        <f>'scoring adjustment'!G8</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f>'scoring adjustment'!E9</f>
-        <v>Accountant</v>
-      </c>
-      <c r="B8" s="3">
-        <f>'scoring adjustment'!G9</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>'scoring adjustment'!E10</f>
-        <v>Business Analyst</v>
-      </c>
-      <c r="B9" s="3">
-        <f>'scoring adjustment'!G10</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f>'scoring adjustment'!E11</f>
-        <v>Executive</v>
-      </c>
-      <c r="B10" s="3">
-        <f>'scoring adjustment'!G11</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f>'scoring adjustment'!E12</f>
-        <v>Secretary</v>
-      </c>
-      <c r="B11" s="3">
-        <f>'scoring adjustment'!G12</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f>'scoring adjustment'!E13</f>
-        <v>Personal Assistant</v>
-      </c>
-      <c r="B12" s="3">
-        <f>'scoring adjustment'!G13</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f>'scoring adjustment'!E14</f>
-        <v>Technician</v>
-      </c>
-      <c r="B13" s="3">
-        <f>'scoring adjustment'!G14</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <f>'scoring adjustment'!E15</f>
-        <v>Others</v>
-      </c>
-      <c r="B14" s="3">
-        <f>'scoring adjustment'!G15</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0B83DB-BB65-45DE-AD9A-34DA85668F66}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>'scoring adjustment'!K3</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>'scoring adjustment'!I4</f>
-        <v>Pos Laju</v>
-      </c>
-      <c r="B3">
-        <f>'scoring adjustment'!K4</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>'scoring adjustment'!I5</f>
-        <v>Gdex</v>
-      </c>
-      <c r="B4">
-        <f>'scoring adjustment'!K5</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>'scoring adjustment'!I6</f>
-        <v>Fedex</v>
-      </c>
-      <c r="B5">
-        <f>'scoring adjustment'!K6</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>'scoring adjustment'!I7</f>
-        <v>J&amp;T</v>
-      </c>
-      <c r="B6">
-        <f>'scoring adjustment'!K7</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f>'scoring adjustment'!I8</f>
-        <v>Citylink</v>
-      </c>
-      <c r="B7">
-        <f>'scoring adjustment'!K8</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f>'scoring adjustment'!I9</f>
-        <v>Easyparcel</v>
-      </c>
-      <c r="B8">
-        <f>'scoring adjustment'!K9</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f>'scoring adjustment'!I10</f>
-        <v>Pgeon</v>
-      </c>
-      <c r="B9">
-        <f>'scoring adjustment'!K10</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f>'scoring adjustment'!I11</f>
-        <v>Ninjavan</v>
-      </c>
-      <c r="B10">
-        <f>'scoring adjustment'!K11</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f>'scoring adjustment'!I12</f>
-        <v>Lalamove</v>
-      </c>
-      <c r="B11">
-        <f>'scoring adjustment'!K12</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f>'scoring adjustment'!I13</f>
-        <v>Others</v>
-      </c>
-      <c r="B12">
-        <f>'scoring adjustment'!K13</f>
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF780DE-784D-4A69-8B98-E103B0FEB401}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>'scoring adjustment'!C39</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f>'scoring adjustment'!A40</f>
-        <v>All Null</v>
-      </c>
-      <c r="B3">
-        <f>'scoring adjustment'!C40</f>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f>'scoring adjustment'!A41</f>
-        <v>Null email</v>
-      </c>
-      <c r="B4">
-        <f>'scoring adjustment'!C41</f>
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f>'scoring adjustment'!A42</f>
-        <v>Null phone no.</v>
-      </c>
-      <c r="B5">
-        <f>'scoring adjustment'!C42</f>
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f>'scoring adjustment'!A43</f>
-        <v>Have both</v>
-      </c>
-      <c r="B6">
-        <f>'scoring adjustment'!C43</f>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7D6719-ECED-4193-8F1E-6CF4287CC736}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,43 +1200,43 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" s="12">
         <v>0.3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G3" s="12">
         <v>0.2</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K3" s="12">
         <v>0.2</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="O3" s="12">
         <v>0.1</v>
@@ -1842,25 +1244,25 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7">
-        <v>100</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
       <c r="G4" s="7">
         <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K4" s="7">
         <v>100</v>
       </c>
       <c r="M4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="O4" s="7">
         <v>100</v>
@@ -1874,19 +1276,19 @@
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G5" s="7">
         <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K5" s="7">
         <v>100</v>
       </c>
       <c r="M5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="O5" s="7">
         <v>100</v>
@@ -1894,25 +1296,25 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C6" s="7">
         <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" s="7">
         <v>100</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K6" s="7">
         <v>100</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O6" s="14">
         <v>100</v>
@@ -1926,19 +1328,19 @@
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G7" s="7">
         <v>100</v>
       </c>
       <c r="I7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K7" s="7">
         <v>80</v>
       </c>
       <c r="M7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="O7" s="7">
         <v>80</v>
@@ -1946,25 +1348,25 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C8" s="7">
         <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G8" s="7">
         <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K8" s="7">
         <v>80</v>
       </c>
       <c r="M8" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="O8" s="7">
         <v>80</v>
@@ -1978,19 +1380,19 @@
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G9" s="7">
         <v>80</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K9" s="7">
         <v>80</v>
       </c>
       <c r="M9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="O9" s="7">
         <v>60</v>
@@ -1998,25 +1400,25 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C10" s="7">
         <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G10" s="7">
         <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K10" s="7">
         <v>80</v>
       </c>
       <c r="M10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="O10" s="7">
         <v>60</v>
@@ -2024,25 +1426,25 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C11" s="7">
         <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G11" s="7">
         <v>70</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K11" s="7">
         <v>80</v>
       </c>
       <c r="M11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="O11" s="7">
         <v>60</v>
@@ -2050,25 +1452,25 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="C12" s="7">
         <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G12" s="7">
         <v>60</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K12" s="7">
         <v>80</v>
       </c>
       <c r="M12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="O12" s="7">
         <v>50</v>
@@ -2076,25 +1478,25 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="7">
         <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G13" s="7">
         <v>60</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K13" s="7">
         <v>100</v>
       </c>
       <c r="M13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O13" s="7">
         <v>-10</v>
@@ -2102,19 +1504,19 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C14" s="7">
         <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G14" s="7">
         <v>50</v>
       </c>
       <c r="M14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="O14" s="7">
         <v>-10</v>
@@ -2122,13 +1524,13 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="C15" s="7">
         <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G15" s="7">
         <v>0</v>
@@ -2136,7 +1538,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C16" s="7">
         <v>80</v>
@@ -2144,7 +1546,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C17" s="7">
         <v>60</v>
@@ -2160,7 +1562,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C19" s="7">
         <v>40</v>
@@ -2168,7 +1570,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C20" s="7">
         <v>10</v>
@@ -2176,15 +1578,15 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21" s="7">
-        <v>100</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C22" s="7">
         <v>40</v>
@@ -2193,28 +1595,28 @@
     <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C25" s="12">
         <v>0.05</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G25" s="13">
         <v>0.05</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K25" s="13">
         <v>0.1</v>
@@ -2222,19 +1624,22 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C26" s="7">
         <v>100</v>
       </c>
       <c r="E26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="15">
+        <v>80</v>
+      </c>
+      <c r="G26">
+        <v>100</v>
+      </c>
+      <c r="I26" t="s">
         <v>104</v>
-      </c>
-      <c r="G26">
-        <v>100</v>
-      </c>
-      <c r="I26" t="s">
-        <v>108</v>
       </c>
       <c r="K26">
         <v>100</v>
@@ -2242,19 +1647,22 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C27" s="7">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="F27" s="15">
+        <v>100</v>
       </c>
       <c r="G27">
         <v>50</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="K27">
         <v>80</v>
@@ -2262,19 +1670,22 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C28" s="7">
         <v>10</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="F28" s="15">
+        <v>100</v>
       </c>
       <c r="G28">
         <v>20</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K28">
         <v>50</v>
@@ -2282,19 +1693,22 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C29" s="7">
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+      <c r="F29" s="15">
+        <v>70</v>
       </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K29">
         <v>20</v>
@@ -2302,13 +1716,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C30" s="7">
         <v>-50</v>
       </c>
       <c r="I30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K30">
         <v>10</v>
@@ -2316,7 +1730,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" s="7">
         <v>0</v>
@@ -2324,7 +1738,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B34" s="10">
         <f>C3+G25+K25+C25+O3+G3+K3</f>
@@ -2333,150 +1747,150 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C39" s="12">
         <v>1</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G39" s="13">
         <v>0.1</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C40" s="7">
         <v>-100</v>
       </c>
       <c r="E40" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J40" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C41" s="9">
         <v>-5</v>
       </c>
       <c r="E41" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G41">
         <v>-20</v>
       </c>
       <c r="I41" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J41" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C42" s="7">
         <v>-20</v>
       </c>
       <c r="E42" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G42">
         <v>-50</v>
       </c>
       <c r="I42" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C43" s="7">
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G43">
         <v>-100</v>
       </c>
       <c r="I43" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B45" s="7">
         <f t="shared" ref="B45:B54" si="0">LEN(A45)</f>
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E47">
         <f>LEN(D47)</f>
@@ -2485,14 +1899,14 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E48">
         <f>LEN(D48)</f>
@@ -2501,7 +1915,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
@@ -2510,7 +1924,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
@@ -2519,7 +1933,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B51" s="7">
         <f t="shared" si="0"/>
@@ -2528,7 +1942,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
@@ -2537,7 +1951,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
@@ -2546,7 +1960,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
@@ -2555,7 +1969,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B55">
         <f>LEN(A55)</f>
@@ -2564,7 +1978,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B56" s="7">
         <f t="shared" ref="B56:B66" si="1">LEN(A56)</f>
@@ -2573,7 +1987,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B57">
         <f t="shared" si="1"/>
@@ -2582,7 +1996,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B58">
         <f t="shared" si="1"/>
@@ -2591,7 +2005,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B59">
         <f t="shared" si="1"/>
@@ -2600,7 +2014,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B60">
         <f t="shared" si="1"/>
@@ -2609,7 +2023,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B61" s="7">
         <f t="shared" si="1"/>
@@ -2618,7 +2032,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B62">
         <f t="shared" si="1"/>
@@ -2627,7 +2041,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B63">
         <f t="shared" si="1"/>
@@ -2636,7 +2050,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B64">
         <f t="shared" si="1"/>
@@ -2645,7 +2059,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B65">
         <f t="shared" si="1"/>
@@ -2654,7 +2068,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B66" s="7">
         <f t="shared" si="1"/>
@@ -2665,4 +2079,612 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C4B6C5-2FF9-429D-B1B8-6831F1847B16}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB39EB3-5C8D-47CC-9F86-693F4D81C503}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>'scoring adjustment'!C25</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>'scoring adjustment'!A26</f>
+        <v>B2B</v>
+      </c>
+      <c r="B3">
+        <f>'scoring adjustment'!C26</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>'scoring adjustment'!A27</f>
+        <v>B2C</v>
+      </c>
+      <c r="B4">
+        <f>'scoring adjustment'!C27</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>'scoring adjustment'!A28</f>
+        <v>Subscription based</v>
+      </c>
+      <c r="B5">
+        <f>'scoring adjustment'!C28</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>'scoring adjustment'!A29</f>
+        <v>On demand</v>
+      </c>
+      <c r="B6">
+        <f>'scoring adjustment'!C29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>'scoring adjustment'!A30</f>
+        <v>Non-profit</v>
+      </c>
+      <c r="B7">
+        <f>'scoring adjustment'!C30</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>'scoring adjustment'!A31</f>
+        <v>Others</v>
+      </c>
+      <c r="B8">
+        <f>'scoring adjustment'!C31</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0957A0A-2F34-4B4E-B07C-7D49062D6D9E}">
+  <dimension ref="C1:D13"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <f>'scoring adjustment'!O3</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C3" t="str">
+        <f>'scoring adjustment'!M4</f>
+        <v>Signup Page</v>
+      </c>
+      <c r="D3" s="3">
+        <f>'scoring adjustment'!O4</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C4" t="str">
+        <f>'scoring adjustment'!M5</f>
+        <v>Landing page</v>
+      </c>
+      <c r="D4" s="3">
+        <f>'scoring adjustment'!O5</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C5" t="str">
+        <f>'scoring adjustment'!M6</f>
+        <v>Exhibition</v>
+      </c>
+      <c r="D5" s="3">
+        <f>'scoring adjustment'!O6</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="str">
+        <f>'scoring adjustment'!M7</f>
+        <v>Referrals</v>
+      </c>
+      <c r="D6" s="3">
+        <f>'scoring adjustment'!O7</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="str">
+        <f>'scoring adjustment'!M8</f>
+        <v>LinkedIn</v>
+      </c>
+      <c r="D7" s="3">
+        <f>'scoring adjustment'!O8</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C8" t="str">
+        <f>'scoring adjustment'!M9</f>
+        <v>Facebook</v>
+      </c>
+      <c r="D8" s="3">
+        <f>'scoring adjustment'!O9</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C9" t="str">
+        <f>'scoring adjustment'!M10</f>
+        <v>Twitter</v>
+      </c>
+      <c r="D9" s="3">
+        <f>'scoring adjustment'!O10</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="str">
+        <f>'scoring adjustment'!M11</f>
+        <v>Blog</v>
+      </c>
+      <c r="D10" s="3">
+        <f>'scoring adjustment'!O11</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C11" t="str">
+        <f>'scoring adjustment'!M12</f>
+        <v>Ex Database</v>
+      </c>
+      <c r="D11" s="3">
+        <f>'scoring adjustment'!O12</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="str">
+        <f>'scoring adjustment'!M13</f>
+        <v>Market Data</v>
+      </c>
+      <c r="D12" s="3">
+        <f>'scoring adjustment'!O13</f>
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="str">
+        <f>'scoring adjustment'!M14</f>
+        <v>Others</v>
+      </c>
+      <c r="D13" s="3">
+        <f>'scoring adjustment'!O14</f>
+        <v>-10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F4B3E4-2AA4-42DF-A18B-2369BF556360}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <f>'scoring adjustment'!G3</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>'scoring adjustment'!E4</f>
+        <v>CEO</v>
+      </c>
+      <c r="B3" s="3">
+        <f>'scoring adjustment'!G4</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>'scoring adjustment'!E5</f>
+        <v>Sales</v>
+      </c>
+      <c r="B4" s="3">
+        <f>'scoring adjustment'!G5</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>'scoring adjustment'!E6</f>
+        <v>Logistics</v>
+      </c>
+      <c r="B5" s="3">
+        <f>'scoring adjustment'!G6</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>'scoring adjustment'!E7</f>
+        <v>Director</v>
+      </c>
+      <c r="B6" s="3">
+        <f>'scoring adjustment'!G7</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>'scoring adjustment'!E8</f>
+        <v>Manager</v>
+      </c>
+      <c r="B7" s="3">
+        <f>'scoring adjustment'!G8</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>'scoring adjustment'!E9</f>
+        <v>Accountant</v>
+      </c>
+      <c r="B8" s="3">
+        <f>'scoring adjustment'!G9</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>'scoring adjustment'!E10</f>
+        <v>Business Analyst</v>
+      </c>
+      <c r="B9" s="3">
+        <f>'scoring adjustment'!G10</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>'scoring adjustment'!E11</f>
+        <v>Executive</v>
+      </c>
+      <c r="B10" s="3">
+        <f>'scoring adjustment'!G11</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>'scoring adjustment'!E12</f>
+        <v>Secretary</v>
+      </c>
+      <c r="B11" s="3">
+        <f>'scoring adjustment'!G12</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>'scoring adjustment'!E13</f>
+        <v>Personal Assistant</v>
+      </c>
+      <c r="B12" s="3">
+        <f>'scoring adjustment'!G13</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="str">
+        <f>'scoring adjustment'!E14</f>
+        <v>Technician</v>
+      </c>
+      <c r="B13" s="3">
+        <f>'scoring adjustment'!G14</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="str">
+        <f>'scoring adjustment'!E15</f>
+        <v>Others</v>
+      </c>
+      <c r="B14" s="3">
+        <f>'scoring adjustment'!G15</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0B83DB-BB65-45DE-AD9A-34DA85668F66}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>'scoring adjustment'!K3</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>'scoring adjustment'!I4</f>
+        <v>Pos Laju</v>
+      </c>
+      <c r="B3">
+        <f>'scoring adjustment'!K4</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>'scoring adjustment'!I5</f>
+        <v>Gdex</v>
+      </c>
+      <c r="B4">
+        <f>'scoring adjustment'!K5</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>'scoring adjustment'!I6</f>
+        <v>Fedex</v>
+      </c>
+      <c r="B5">
+        <f>'scoring adjustment'!K6</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>'scoring adjustment'!I7</f>
+        <v>J&amp;T</v>
+      </c>
+      <c r="B6">
+        <f>'scoring adjustment'!K7</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="str">
+        <f>'scoring adjustment'!I8</f>
+        <v>Citylink</v>
+      </c>
+      <c r="B7">
+        <f>'scoring adjustment'!K8</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="str">
+        <f>'scoring adjustment'!I9</f>
+        <v>Easyparcel</v>
+      </c>
+      <c r="B8">
+        <f>'scoring adjustment'!K9</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="str">
+        <f>'scoring adjustment'!I10</f>
+        <v>Pgeon</v>
+      </c>
+      <c r="B9">
+        <f>'scoring adjustment'!K10</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="str">
+        <f>'scoring adjustment'!I11</f>
+        <v>Ninjavan</v>
+      </c>
+      <c r="B10">
+        <f>'scoring adjustment'!K11</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="str">
+        <f>'scoring adjustment'!I12</f>
+        <v>Lalamove</v>
+      </c>
+      <c r="B11">
+        <f>'scoring adjustment'!K12</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="str">
+        <f>'scoring adjustment'!I13</f>
+        <v>Others</v>
+      </c>
+      <c r="B12">
+        <f>'scoring adjustment'!K13</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF780DE-784D-4A69-8B98-E103B0FEB401}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>'scoring adjustment'!C39</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>'scoring adjustment'!A40</f>
+        <v>All Null</v>
+      </c>
+      <c r="B3">
+        <f>'scoring adjustment'!C40</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>'scoring adjustment'!A41</f>
+        <v>Null email</v>
+      </c>
+      <c r="B4">
+        <f>'scoring adjustment'!C41</f>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="str">
+        <f>'scoring adjustment'!A42</f>
+        <v>Null phone no.</v>
+      </c>
+      <c r="B5">
+        <f>'scoring adjustment'!C42</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="str">
+        <f>'scoring adjustment'!A43</f>
+        <v>Have both</v>
+      </c>
+      <c r="B6">
+        <f>'scoring adjustment'!C43</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update scoring adjustment excel
</commit_message>
<xml_diff>
--- a/compile/data/weighted_adjustment.xlsx
+++ b/compile/data/weighted_adjustment.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\group\compile\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ssyazz\python\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52103E36-176D-43F8-8DF4-6C2EC6BA585E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9D2620-827C-4EDE-A42F-0A86C8AAB6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FD519D9B-FD8C-4B05-8A2B-BFB2B0A3DB28}"/>
   </bookViews>
   <sheets>
     <sheet name="industry" sheetId="1" r:id="rId1"/>
-    <sheet name="creation_date" sheetId="2" r:id="rId2"/>
+    <sheet name="employee_count" sheetId="3" r:id="rId2"/>
     <sheet name="scoring adjustment" sheetId="8" r:id="rId3"/>
-    <sheet name="employee_count" sheetId="3" r:id="rId4"/>
-    <sheet name="physical_channel" sheetId="4" r:id="rId5"/>
-    <sheet name="lead_source" sheetId="5" r:id="rId6"/>
-    <sheet name="designation" sheetId="6" r:id="rId7"/>
-    <sheet name="competitor" sheetId="9" r:id="rId8"/>
-    <sheet name="contact_score" sheetId="7" r:id="rId9"/>
+    <sheet name="physical_channel" sheetId="4" r:id="rId4"/>
+    <sheet name="lead_source" sheetId="5" r:id="rId5"/>
+    <sheet name="designation" sheetId="6" r:id="rId6"/>
+    <sheet name="competitor" sheetId="9" r:id="rId7"/>
+    <sheet name="contact_score" sheetId="7" r:id="rId8"/>
+    <sheet name="creation_date" sheetId="2" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'scoring adjustment'!$C$3</definedName>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="127">
   <si>
     <t>weightage</t>
   </si>
@@ -536,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -557,6 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1095,16 +1096,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7B9016-79F5-47B1-AF6F-53603DC8316B}">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C4B6C5-2FF9-429D-B1B8-6831F1847B16}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1112,65 +1113,50 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <f>'scoring adjustment'!G39</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <f>'scoring adjustment'!G25</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>249</v>
+      </c>
+      <c r="B3">
+        <f>'scoring adjustment'!G26</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>250</v>
+      </c>
+      <c r="B4">
+        <f>'scoring adjustment'!G27</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <f>'scoring adjustment'!G28</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>10</v>
       </c>
-      <c r="B3">
-        <f>'scoring adjustment'!G40</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <f>'scoring adjustment'!G41</f>
-        <v>-20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>90</v>
-      </c>
-      <c r="B5">
-        <f>'scoring adjustment'!G42</f>
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>89</v>
-      </c>
       <c r="B6">
-        <f>'scoring adjustment'!G43</f>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F18" s="2"/>
+        <f>'scoring adjustment'!G29</f>
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1181,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E7D6719-ECED-4193-8F1E-6CF4287CC736}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1609,7 +1595,7 @@
       <c r="F25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="12">
         <v>0.05</v>
       </c>
       <c r="I25" s="4" t="s">
@@ -1632,10 +1618,8 @@
       <c r="E26" t="s">
         <v>100</v>
       </c>
-      <c r="F26" s="15">
-        <v>80</v>
-      </c>
-      <c r="G26">
+      <c r="F26" s="15"/>
+      <c r="G26" s="7">
         <v>100</v>
       </c>
       <c r="I26" t="s">
@@ -1655,11 +1639,9 @@
       <c r="E27" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="15">
-        <v>100</v>
-      </c>
-      <c r="G27">
-        <v>50</v>
+      <c r="F27" s="15"/>
+      <c r="G27" s="7">
+        <v>100</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>103</v>
@@ -1678,11 +1660,9 @@
       <c r="E28" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="15">
-        <v>100</v>
-      </c>
-      <c r="G28">
-        <v>20</v>
+      <c r="F28" s="15"/>
+      <c r="G28" s="7">
+        <v>100</v>
       </c>
       <c r="I28" s="8" t="s">
         <v>102</v>
@@ -1701,11 +1681,9 @@
       <c r="E29" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="15"/>
+      <c r="G29" s="7">
         <v>70</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
       </c>
       <c r="I29" s="8" t="s">
         <v>101</v>
@@ -1767,7 +1745,7 @@
       <c r="F39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="13">
         <v>0.1</v>
       </c>
       <c r="I39" s="5" t="s">
@@ -1787,7 +1765,7 @@
       <c r="E40" t="s">
         <v>22</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40">
         <v>0</v>
       </c>
       <c r="I40" t="s">
@@ -1807,7 +1785,7 @@
       <c r="E41" t="s">
         <v>23</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41">
         <v>-20</v>
       </c>
       <c r="I41" t="s">
@@ -1827,7 +1805,7 @@
       <c r="E42" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42">
         <v>-50</v>
       </c>
       <c r="I42" t="s">
@@ -1847,7 +1825,7 @@
       <c r="E43" t="s">
         <v>25</v>
       </c>
-      <c r="G43" s="7">
+      <c r="G43">
         <v>-100</v>
       </c>
       <c r="I43" t="s">
@@ -2082,18 +2060,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82C4B6C5-2FF9-429D-B1B8-6831F1847B16}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB39EB3-5C8D-47CC-9F86-693F4D81C503}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -2185,7 +2151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0957A0A-2F34-4B4E-B07C-7D49062D6D9E}">
   <dimension ref="C1:D13"/>
   <sheetViews>
@@ -2330,7 +2296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F4B3E4-2AA4-42DF-A18B-2369BF556360}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -2482,7 +2448,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B0B83DB-BB65-45DE-AD9A-34DA85668F66}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -2614,7 +2580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF780DE-784D-4A69-8B98-E103B0FEB401}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2687,4 +2653,87 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7B9016-79F5-47B1-AF6F-53603DC8316B}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>'scoring adjustment'!G39</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <f>'scoring adjustment'!G40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <f>'scoring adjustment'!G41</f>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>90</v>
+      </c>
+      <c r="B5">
+        <f>'scoring adjustment'!G42</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>89</v>
+      </c>
+      <c r="B6">
+        <f>'scoring adjustment'!G43</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>